<commit_message>
Retraining the RAAL Production model
</commit_message>
<xml_diff>
--- a/Solina/Consumption/Results/Results_Consumption_Solina.xlsx
+++ b/Solina/Consumption/Results/Results_Consumption_Solina.xlsx
@@ -443,228 +443,228 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>0.204</v>
+        <v>0.211</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>10</v>
       </c>
       <c r="C3" t="n">
-        <v>0.203</v>
+        <v>0.212</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>0.199</v>
+        <v>0.223</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>0.189</v>
+        <v>0.216</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>13</v>
       </c>
       <c r="C6" t="n">
-        <v>0.182</v>
+        <v>0.211</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.167</v>
+        <v>0.205</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>15</v>
       </c>
       <c r="C8" t="n">
-        <v>0.168</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>16</v>
       </c>
       <c r="C9" t="n">
-        <v>0.156</v>
+        <v>0.178</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>17</v>
       </c>
       <c r="C10" t="n">
-        <v>0.139</v>
+        <v>0.164</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>18</v>
       </c>
       <c r="C11" t="n">
-        <v>0.137</v>
+        <v>0.153</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>19</v>
       </c>
       <c r="C12" t="n">
-        <v>0.14</v>
+        <v>0.145</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>20</v>
       </c>
       <c r="C13" t="n">
-        <v>0.139</v>
+        <v>0.142</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>21</v>
       </c>
       <c r="C14" t="n">
-        <v>0.135</v>
+        <v>0.139</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>22</v>
       </c>
       <c r="C15" t="n">
-        <v>0.118</v>
+        <v>0.121</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>23</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1</v>
+        <v>0.103</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>0.091</v>
+        <v>0.092</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>0.08799999999999999</v>
+        <v>0.089</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -677,46 +677,46 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>3</v>
       </c>
       <c r="C20" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.08500000000000001</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B21" t="n">
         <v>4</v>
       </c>
       <c r="C21" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.08500000000000001</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>5</v>
       </c>
       <c r="C22" t="n">
-        <v>0.09</v>
+        <v>0.08799999999999999</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -729,7 +729,7 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -742,33 +742,33 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B25" t="n">
         <v>8</v>
       </c>
       <c r="C25" t="n">
-        <v>0.09</v>
+        <v>0.091</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B26" t="n">
         <v>9</v>
       </c>
       <c r="C26" t="n">
-        <v>0.089</v>
+        <v>0.091</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -781,189 +781,189 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B28" t="n">
         <v>11</v>
       </c>
       <c r="C28" t="n">
-        <v>0.089</v>
+        <v>0.08699999999999999</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B29" t="n">
         <v>12</v>
       </c>
       <c r="C29" t="n">
-        <v>0.113</v>
+        <v>0.091</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B30" t="n">
         <v>13</v>
       </c>
       <c r="C30" t="n">
-        <v>0.11</v>
+        <v>0.089</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B31" t="n">
         <v>14</v>
       </c>
       <c r="C31" t="n">
-        <v>0.109</v>
+        <v>0.08799999999999999</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B32" t="n">
         <v>15</v>
       </c>
       <c r="C32" t="n">
-        <v>0.107</v>
+        <v>0.08799999999999999</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B33" t="n">
         <v>16</v>
       </c>
       <c r="C33" t="n">
-        <v>0.09</v>
+        <v>0.08400000000000001</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B34" t="n">
         <v>17</v>
       </c>
       <c r="C34" t="n">
-        <v>0.08</v>
+        <v>0.08599999999999999</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B35" t="n">
         <v>18</v>
       </c>
       <c r="C35" t="n">
-        <v>0.074</v>
+        <v>0.079</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B36" t="n">
         <v>19</v>
       </c>
       <c r="C36" t="n">
-        <v>0.076</v>
+        <v>0.079</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B37" t="n">
         <v>20</v>
       </c>
       <c r="C37" t="n">
-        <v>0.076</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B38" t="n">
         <v>21</v>
       </c>
       <c r="C38" t="n">
-        <v>0.075</v>
+        <v>0.078</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B39" t="n">
         <v>22</v>
       </c>
       <c r="C39" t="n">
-        <v>0.073</v>
+        <v>0.076</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="B40" t="n">
         <v>23</v>
       </c>
       <c r="C40" t="n">
-        <v>0.07099999999999999</v>
+        <v>0.074</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B41" t="n">
         <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.08699999999999999</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -976,7 +976,7 @@
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -989,7 +989,7 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1002,267 +1002,267 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B45" t="n">
         <v>4</v>
       </c>
       <c r="C45" t="n">
-        <v>0.081</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B46" t="n">
         <v>5</v>
       </c>
       <c r="C46" t="n">
-        <v>0.083</v>
+        <v>0.082</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B47" t="n">
         <v>6</v>
       </c>
       <c r="C47" t="n">
-        <v>0.083</v>
+        <v>0.082</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B48" t="n">
         <v>7</v>
       </c>
       <c r="C48" t="n">
-        <v>0.082</v>
+        <v>0.083</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B49" t="n">
         <v>8</v>
       </c>
       <c r="C49" t="n">
-        <v>0.08</v>
+        <v>0.082</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B50" t="n">
         <v>9</v>
       </c>
       <c r="C50" t="n">
-        <v>0.092</v>
+        <v>0.081</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B51" t="n">
         <v>10</v>
       </c>
       <c r="C51" t="n">
-        <v>0.08400000000000001</v>
+        <v>0.081</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B52" t="n">
         <v>11</v>
       </c>
       <c r="C52" t="n">
-        <v>0.09</v>
+        <v>0.081</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B53" t="n">
         <v>12</v>
       </c>
       <c r="C53" t="n">
-        <v>0.08500000000000001</v>
+        <v>0.083</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B54" t="n">
         <v>13</v>
       </c>
       <c r="C54" t="n">
-        <v>0.092</v>
+        <v>0.08599999999999999</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B55" t="n">
         <v>14</v>
       </c>
       <c r="C55" t="n">
-        <v>0.09</v>
+        <v>0.08500000000000001</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B56" t="n">
         <v>15</v>
       </c>
       <c r="C56" t="n">
-        <v>0.089</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B57" t="n">
         <v>16</v>
       </c>
       <c r="C57" t="n">
-        <v>0.078</v>
+        <v>0.08799999999999999</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B58" t="n">
         <v>17</v>
       </c>
       <c r="C58" t="n">
-        <v>0.079</v>
+        <v>0.08699999999999999</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B59" t="n">
         <v>18</v>
       </c>
       <c r="C59" t="n">
-        <v>0.07199999999999999</v>
+        <v>0.081</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B60" t="n">
         <v>19</v>
       </c>
       <c r="C60" t="n">
-        <v>0.07199999999999999</v>
+        <v>0.083</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B61" t="n">
         <v>20</v>
       </c>
       <c r="C61" t="n">
-        <v>0.073</v>
+        <v>0.077</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B62" t="n">
         <v>21</v>
       </c>
       <c r="C62" t="n">
-        <v>0.073</v>
+        <v>0.076</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B63" t="n">
         <v>22</v>
       </c>
       <c r="C63" t="n">
-        <v>0.07199999999999999</v>
+        <v>0.075</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-14</t>
         </is>
       </c>
       <c r="B64" t="n">
         <v>23</v>
       </c>
       <c r="C64" t="n">
-        <v>0.074</v>
+        <v>0.076</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1275,7 +1275,7 @@
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1288,7 +1288,7 @@
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1301,7 +1301,7 @@
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1314,7 +1314,7 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1327,7 +1327,7 @@
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1340,98 +1340,98 @@
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B71" t="n">
         <v>6</v>
       </c>
       <c r="C71" t="n">
-        <v>0.146</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B72" t="n">
         <v>7</v>
       </c>
       <c r="C72" t="n">
-        <v>0.21</v>
+        <v>0.183</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B73" t="n">
         <v>8</v>
       </c>
       <c r="C73" t="n">
-        <v>0.239</v>
+        <v>0.227</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B74" t="n">
         <v>9</v>
       </c>
       <c r="C74" t="n">
-        <v>0.248</v>
+        <v>0.244</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B75" t="n">
         <v>10</v>
       </c>
       <c r="C75" t="n">
-        <v>0.256</v>
+        <v>0.246</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B76" t="n">
         <v>11</v>
       </c>
       <c r="C76" t="n">
-        <v>0.261</v>
+        <v>0.259</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B77" t="n">
         <v>12</v>
       </c>
       <c r="C77" t="n">
-        <v>0.261</v>
+        <v>0.271</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1444,553 +1444,553 @@
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B79" t="n">
         <v>14</v>
       </c>
       <c r="C79" t="n">
-        <v>0.251</v>
+        <v>0.248</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B80" t="n">
         <v>15</v>
       </c>
       <c r="C80" t="n">
-        <v>0.245</v>
+        <v>0.241</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B81" t="n">
         <v>16</v>
       </c>
       <c r="C81" t="n">
-        <v>0.219</v>
+        <v>0.226</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B82" t="n">
         <v>17</v>
       </c>
       <c r="C82" t="n">
-        <v>0.197</v>
+        <v>0.217</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B83" t="n">
         <v>18</v>
       </c>
       <c r="C83" t="n">
-        <v>0.178</v>
+        <v>0.201</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B84" t="n">
         <v>19</v>
       </c>
       <c r="C84" t="n">
-        <v>0.176</v>
+        <v>0.195</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B85" t="n">
         <v>20</v>
       </c>
       <c r="C85" t="n">
-        <v>0.178</v>
+        <v>0.191</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B86" t="n">
         <v>21</v>
       </c>
       <c r="C86" t="n">
-        <v>0.177</v>
+        <v>0.186</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B87" t="n">
         <v>22</v>
       </c>
       <c r="C87" t="n">
-        <v>0.159</v>
+        <v>0.173</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-15</t>
         </is>
       </c>
       <c r="B88" t="n">
         <v>23</v>
       </c>
       <c r="C88" t="n">
-        <v>0.137</v>
+        <v>0.136</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B89" t="n">
         <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>0.114</v>
+        <v>0.115</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B90" t="n">
         <v>1</v>
       </c>
       <c r="C90" t="n">
-        <v>0.103</v>
+        <v>0.111</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B91" t="n">
         <v>2</v>
       </c>
       <c r="C91" t="n">
-        <v>0.095</v>
+        <v>0.107</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B92" t="n">
         <v>3</v>
       </c>
       <c r="C92" t="n">
-        <v>0.094</v>
+        <v>0.107</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B93" t="n">
         <v>4</v>
       </c>
       <c r="C93" t="n">
-        <v>0.095</v>
+        <v>0.105</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B94" t="n">
         <v>5</v>
       </c>
       <c r="C94" t="n">
-        <v>0.101</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B95" t="n">
         <v>6</v>
       </c>
       <c r="C95" t="n">
-        <v>0.14</v>
+        <v>0.155</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B96" t="n">
         <v>7</v>
       </c>
       <c r="C96" t="n">
-        <v>0.188</v>
+        <v>0.204</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B97" t="n">
         <v>8</v>
       </c>
       <c r="C97" t="n">
-        <v>0.221</v>
+        <v>0.234</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B98" t="n">
         <v>9</v>
       </c>
       <c r="C98" t="n">
-        <v>0.232</v>
+        <v>0.243</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B99" t="n">
         <v>10</v>
       </c>
       <c r="C99" t="n">
-        <v>0.235</v>
+        <v>0.242</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B100" t="n">
         <v>11</v>
       </c>
       <c r="C100" t="n">
-        <v>0.225</v>
+        <v>0.241</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B101" t="n">
         <v>12</v>
       </c>
       <c r="C101" t="n">
-        <v>0.224</v>
+        <v>0.239</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B102" t="n">
         <v>13</v>
       </c>
       <c r="C102" t="n">
-        <v>0.215</v>
+        <v>0.241</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B103" t="n">
         <v>14</v>
       </c>
       <c r="C103" t="n">
-        <v>0.203</v>
+        <v>0.238</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B104" t="n">
         <v>15</v>
       </c>
       <c r="C104" t="n">
-        <v>0.2</v>
+        <v>0.234</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B105" t="n">
         <v>16</v>
       </c>
       <c r="C105" t="n">
-        <v>0.189</v>
+        <v>0.206</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B106" t="n">
         <v>17</v>
       </c>
       <c r="C106" t="n">
-        <v>0.176</v>
+        <v>0.182</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B107" t="n">
         <v>18</v>
       </c>
       <c r="C107" t="n">
-        <v>0.17</v>
+        <v>0.175</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B108" t="n">
         <v>19</v>
       </c>
       <c r="C108" t="n">
-        <v>0.174</v>
+        <v>0.178</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B109" t="n">
         <v>20</v>
       </c>
       <c r="C109" t="n">
-        <v>0.17</v>
+        <v>0.175</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B110" t="n">
         <v>21</v>
       </c>
       <c r="C110" t="n">
-        <v>0.167</v>
+        <v>0.171</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B111" t="n">
         <v>22</v>
       </c>
       <c r="C111" t="n">
-        <v>0.141</v>
+        <v>0.149</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="B112" t="n">
         <v>23</v>
       </c>
       <c r="C112" t="n">
-        <v>0.12</v>
+        <v>0.126</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B113" t="n">
         <v>0</v>
       </c>
       <c r="C113" t="n">
-        <v>0.112</v>
+        <v>0.107</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B114" t="n">
         <v>1</v>
       </c>
       <c r="C114" t="n">
-        <v>0.104</v>
+        <v>0.101</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B115" t="n">
         <v>2</v>
       </c>
       <c r="C115" t="n">
-        <v>0.098</v>
+        <v>0.097</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B116" t="n">
         <v>3</v>
       </c>
       <c r="C116" t="n">
-        <v>0.097</v>
+        <v>0.096</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B117" t="n">
         <v>4</v>
       </c>
       <c r="C117" t="n">
-        <v>0.098</v>
+        <v>0.097</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B118" t="n">
         <v>5</v>
       </c>
       <c r="C118" t="n">
-        <v>0.107</v>
+        <v>0.105</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B119" t="n">
         <v>6</v>
       </c>
       <c r="C119" t="n">
-        <v>0.143</v>
+        <v>0.144</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B120" t="n">
         <v>7</v>
       </c>
       <c r="C120" t="n">
-        <v>0.189</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B121" t="n">
@@ -2003,20 +2003,20 @@
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B122" t="n">
         <v>9</v>
       </c>
       <c r="C122" t="n">
-        <v>0.233</v>
+        <v>0.232</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B123" t="n">
@@ -2029,33 +2029,33 @@
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B124" t="n">
         <v>11</v>
       </c>
       <c r="C124" t="n">
-        <v>0.218</v>
+        <v>0.219</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B125" t="n">
         <v>12</v>
       </c>
       <c r="C125" t="n">
-        <v>0.216</v>
+        <v>0.217</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B126" t="n">
@@ -2068,46 +2068,46 @@
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B127" t="n">
         <v>14</v>
       </c>
       <c r="C127" t="n">
-        <v>0.198</v>
+        <v>0.197</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B128" t="n">
         <v>15</v>
       </c>
       <c r="C128" t="n">
-        <v>0.197</v>
+        <v>0.196</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B129" t="n">
         <v>16</v>
       </c>
       <c r="C129" t="n">
-        <v>0.186</v>
+        <v>0.184</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B130" t="n">
@@ -2120,20 +2120,20 @@
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B131" t="n">
         <v>18</v>
       </c>
       <c r="C131" t="n">
-        <v>0.17</v>
+        <v>0.169</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B132" t="n">
@@ -2146,33 +2146,33 @@
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B133" t="n">
         <v>20</v>
       </c>
       <c r="C133" t="n">
-        <v>0.166</v>
+        <v>0.171</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B134" t="n">
         <v>21</v>
       </c>
       <c r="C134" t="n">
-        <v>0.167</v>
+        <v>0.166</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B135" t="n">
@@ -2185,7 +2185,7 @@
     <row r="136">
       <c r="A136" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="B136" t="n">
@@ -2198,59 +2198,59 @@
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B137" t="n">
         <v>0</v>
       </c>
       <c r="C137" t="n">
-        <v>0.109</v>
+        <v>0.113</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B138" t="n">
         <v>1</v>
       </c>
       <c r="C138" t="n">
-        <v>0.102</v>
+        <v>0.105</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B139" t="n">
         <v>2</v>
       </c>
       <c r="C139" t="n">
-        <v>0.099</v>
+        <v>0.101</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B140" t="n">
         <v>3</v>
       </c>
       <c r="C140" t="n">
-        <v>0.097</v>
+        <v>0.098</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B141" t="n">
@@ -2263,150 +2263,150 @@
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B142" t="n">
         <v>5</v>
       </c>
       <c r="C142" t="n">
-        <v>0.107</v>
+        <v>0.104</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B143" t="n">
         <v>6</v>
       </c>
       <c r="C143" t="n">
-        <v>0.144</v>
+        <v>0.143</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B144" t="n">
         <v>7</v>
       </c>
       <c r="C144" t="n">
-        <v>0.189</v>
+        <v>0.187</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B145" t="n">
         <v>8</v>
       </c>
       <c r="C145" t="n">
-        <v>0.222</v>
+        <v>0.221</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B146" t="n">
         <v>9</v>
       </c>
       <c r="C146" t="n">
-        <v>0.231</v>
+        <v>0.228</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B147" t="n">
         <v>10</v>
       </c>
       <c r="C147" t="n">
-        <v>0.231</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B148" t="n">
         <v>11</v>
       </c>
       <c r="C148" t="n">
-        <v>0.222</v>
+        <v>0.215</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B149" t="n">
         <v>12</v>
       </c>
       <c r="C149" t="n">
-        <v>0.221</v>
+        <v>0.218</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B150" t="n">
         <v>13</v>
       </c>
       <c r="C150" t="n">
-        <v>0.216</v>
+        <v>0.203</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B151" t="n">
         <v>14</v>
       </c>
       <c r="C151" t="n">
-        <v>0.201</v>
+        <v>0.196</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B152" t="n">
         <v>15</v>
       </c>
       <c r="C152" t="n">
-        <v>0.199</v>
+        <v>0.193</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B153" t="n">
@@ -2419,46 +2419,46 @@
     <row r="154">
       <c r="A154" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B154" t="n">
         <v>17</v>
       </c>
       <c r="C154" t="n">
-        <v>0.172</v>
+        <v>0.171</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B155" t="n">
         <v>18</v>
       </c>
       <c r="C155" t="n">
-        <v>0.168</v>
+        <v>0.165</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B156" t="n">
         <v>19</v>
       </c>
       <c r="C156" t="n">
-        <v>0.171</v>
+        <v>0.174</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B157" t="n">
@@ -2471,33 +2471,33 @@
     <row r="158">
       <c r="A158" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B158" t="n">
         <v>21</v>
       </c>
       <c r="C158" t="n">
-        <v>0.165</v>
+        <v>0.164</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B159" t="n">
         <v>22</v>
       </c>
       <c r="C159" t="n">
-        <v>0.141</v>
+        <v>0.137</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-18</t>
         </is>
       </c>
       <c r="B160" t="n">
@@ -2510,131 +2510,131 @@
     <row r="161">
       <c r="A161" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-19</t>
         </is>
       </c>
       <c r="B161" t="n">
         <v>0</v>
       </c>
       <c r="C161" t="n">
-        <v>0.105</v>
+        <v>0.103</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-19</t>
         </is>
       </c>
       <c r="B162" t="n">
         <v>1</v>
       </c>
       <c r="C162" t="n">
-        <v>0.099</v>
+        <v>0.096</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-19</t>
         </is>
       </c>
       <c r="B163" t="n">
         <v>2</v>
       </c>
       <c r="C163" t="n">
-        <v>0.095</v>
+        <v>0.093</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-19</t>
         </is>
       </c>
       <c r="B164" t="n">
         <v>3</v>
       </c>
       <c r="C164" t="n">
-        <v>0.094</v>
+        <v>0.091</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-19</t>
         </is>
       </c>
       <c r="B165" t="n">
         <v>4</v>
       </c>
       <c r="C165" t="n">
-        <v>0.095</v>
+        <v>0.094</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-19</t>
         </is>
       </c>
       <c r="B166" t="n">
         <v>5</v>
       </c>
       <c r="C166" t="n">
-        <v>0.101</v>
+        <v>0.106</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-19</t>
         </is>
       </c>
       <c r="B167" t="n">
         <v>6</v>
       </c>
       <c r="C167" t="n">
-        <v>0.136</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-19</t>
         </is>
       </c>
       <c r="B168" t="n">
         <v>7</v>
       </c>
       <c r="C168" t="n">
-        <v>0.182</v>
+        <v>0.181</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-19</t>
         </is>
       </c>
       <c r="B169" t="n">
         <v>8</v>
       </c>
       <c r="C169" t="n">
-        <v>0.203</v>
+        <v>0.201</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-19</t>
         </is>
       </c>
       <c r="B170" t="n">
         <v>9</v>
       </c>
       <c r="C170" t="n">
-        <v>0.212</v>
+        <v>0.213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>